<commit_message>
add trend for compare
</commit_message>
<xml_diff>
--- a/files/export_formats/report_format.xlsx
+++ b/files/export_formats/report_format.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amir\Desktop\m\Paticle_Size_Analyser\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amir\Desktop\m\Paticle_Size_Analyser\files\export_formats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DDB64CF-878F-4872-8F07-6C7F7FC1EC41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AE3EB07-DE94-40A3-8B04-68FFE9989380}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10788" yWindow="1464" windowWidth="12252" windowHeight="9420" xr2:uid="{C9C2E82C-97A0-4E56-8AF9-18415E4F1BF7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{C9C2E82C-97A0-4E56-8AF9-18415E4F1BF7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -270,6 +270,792 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.10344203849518811"/>
+          <c:y val="0.19486111111111112"/>
+          <c:w val="0.89655796150481193"/>
+          <c:h val="0.72088764946048411"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="481569808"/>
+        <c:axId val="481570136"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="481569808"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="481570136"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="481570136"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="481569808"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>289560</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="%">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C5902B95-BDE7-441E-9D2A-8FA7974B335D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -569,15 +1355,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39703DDA-2BAB-4B89-A984-FAF08C9B9286}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="50.44140625" style="2" customWidth="1"/>
     <col min="2" max="2" width="17" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.88671875" style="2" customWidth="1"/>
     <col min="4" max="4" width="12.88671875" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="8.88671875" style="2"/>
   </cols>
@@ -657,5 +1443,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
chart added for export report
</commit_message>
<xml_diff>
--- a/files/export_formats/report_format.xlsx
+++ b/files/export_formats/report_format.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amir\Desktop\m\Paticle_Size_Analyser\files\export_formats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AB02503-F384-428A-A235-D9E99181371D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AF08679-45E0-4C54-A519-676F3A1DEAB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{C9C2E82C-97A0-4E56-8AF9-18415E4F1BF7}"/>
   </bookViews>
@@ -308,14 +308,8 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>TESSS</a:t>
+              <a:t>Grading</a:t>
             </a:r>
-          </a:p>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -360,9 +354,12 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$15</c:f>
+              <c:f>Sheet1!$A$10</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>%RANGE_NAME_HORIZONTAL%</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
@@ -376,93 +373,39 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$A$16</c:f>
+              <c:f>Sheet1!$A$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-7F52-4C12-A5FA-B8EC07B1D31C}"/>
+              <c16:uniqueId val="{00000000-76F9-42BC-84D0-222CE0609796}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
-          <c:showVal val="1"/>
+          <c:showVal val="0"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:overlap val="-25"/>
-        <c:axId val="481569808"/>
-        <c:axId val="481570136"/>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="513678960"/>
+        <c:axId val="513676008"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="481569808"/>
+        <c:axId val="513678960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -504,7 +447,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="481570136"/>
+        <c:crossAx val="513676008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -512,17 +455,58 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="481570136"/>
+        <c:axId val="513676008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="1"/>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="481569808"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="513678960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -534,37 +518,6 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="t"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -1156,23 +1109,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>762000</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>60960</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>3444240</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>289560</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>60960</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>121920</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="%10">
+        <xdr:cNvPr id="5" name="Chart 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C5902B95-BDE7-441E-9D2A-8FA7974B335D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EA82C1F3-550D-4DD4-8F78-46FA392D979F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1492,8 +1445,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39703DDA-2BAB-4B89-A984-FAF08C9B9286}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21.6" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
filter bug fix, camera is in develope
</commit_message>
<xml_diff>
--- a/files/export_formats/report_format.xlsx
+++ b/files/export_formats/report_format.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amir\Desktop\m\Paticle_Size_Analyser\files\export_formats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AF08679-45E0-4C54-A519-676F3A1DEAB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DC44136-70EF-4C96-9C66-747866DC59B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{C9C2E82C-97A0-4E56-8AF9-18415E4F1BF7}"/>
   </bookViews>
@@ -1110,15 +1110,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>3444240</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>91440</xdr:rowOff>
+      <xdr:colOff>213360</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>121920</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>91440</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1445,8 +1445,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39703DDA-2BAB-4B89-A984-FAF08C9B9286}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21.6" x14ac:dyDescent="0.3"/>

</xml_diff>